<commit_message>
add save and restore
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/Stack/Stack_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9FE347-42A9-484F-881B-F7AF16BBA40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640BE905-9E67-214F-B36E-FDA43AC728C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="600" windowWidth="33600" windowHeight="20500" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D968784-9ABC-434B-B612-3087309D1BAB}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,7 +653,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -667,7 +667,7 @@
         <v>13</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
         <v>22</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="E18">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -835,7 +835,7 @@
         <v>22</v>
       </c>
       <c r="E19">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>